<commit_message>
updated the gemini response
</commit_message>
<xml_diff>
--- a/sheets/estimated_bills.xlsx
+++ b/sheets/estimated_bills.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Solar Value 12</t>
+          <t xml:space="preserve"> Simple Rate 12</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -463,10 +463,20 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> e-Saver 10</t>
+          <t xml:space="preserve"> e-Saver 12</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Saver's Choice 12</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Solar Buyback Saver 36</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> Flex Forward</t>
         </is>
@@ -479,28 +489,34 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>207.15</v>
+        <v>29.85</v>
       </c>
       <c r="D2" t="n">
-        <v>287.23</v>
+        <v>37.93</v>
       </c>
       <c r="E2" t="n">
-        <v>155.09</v>
+        <v>22.88</v>
       </c>
       <c r="F2" t="n">
-        <v>239.18</v>
+        <v>33.08</v>
       </c>
       <c r="G2" t="n">
-        <v>203.14</v>
+        <v>29.44</v>
       </c>
       <c r="H2" t="n">
-        <v>129.07</v>
+        <v>22.5</v>
       </c>
       <c r="I2" t="n">
-        <v>136.08</v>
+        <v>24.7</v>
+      </c>
+      <c r="J2" t="n">
+        <v>27.57</v>
+      </c>
+      <c r="K2" t="n">
+        <v>22.68</v>
       </c>
     </row>
     <row r="3">
@@ -510,28 +526,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C3" t="n">
-        <v>29.85</v>
+        <v>49.55</v>
       </c>
       <c r="D3" t="n">
-        <v>37.93</v>
+        <v>65.63</v>
       </c>
       <c r="E3" t="n">
-        <v>24.59</v>
+        <v>35.68</v>
       </c>
       <c r="F3" t="n">
-        <v>33.08</v>
+        <v>55.98</v>
       </c>
       <c r="G3" t="n">
-        <v>29.44</v>
+        <v>48.74</v>
       </c>
       <c r="H3" t="n">
-        <v>19.27</v>
+        <v>37.9</v>
       </c>
       <c r="I3" t="n">
-        <v>22.68</v>
+        <v>39.3</v>
+      </c>
+      <c r="J3" t="n">
+        <v>40.08</v>
+      </c>
+      <c r="K3" t="n">
+        <v>35.28</v>
       </c>
     </row>
     <row r="4">
@@ -541,28 +563,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="C4" t="n">
-        <v>207.15</v>
+        <v>69.25</v>
       </c>
       <c r="D4" t="n">
-        <v>287.23</v>
+        <v>93.33</v>
       </c>
       <c r="E4" t="n">
-        <v>155.09</v>
+        <v>48.48</v>
       </c>
       <c r="F4" t="n">
-        <v>239.18</v>
+        <v>78.88</v>
       </c>
       <c r="G4" t="n">
-        <v>203.14</v>
+        <v>68.04000000000001</v>
       </c>
       <c r="H4" t="n">
-        <v>129.07</v>
+        <v>53.3</v>
       </c>
       <c r="I4" t="n">
-        <v>136.08</v>
+        <v>53.9</v>
+      </c>
+      <c r="J4" t="n">
+        <v>52.58</v>
+      </c>
+      <c r="K4" t="n">
+        <v>47.88</v>
       </c>
     </row>
     <row r="5">
@@ -572,28 +600,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="C5" t="n">
-        <v>29.85</v>
+        <v>88.95</v>
       </c>
       <c r="D5" t="n">
-        <v>37.93</v>
+        <v>121.03</v>
       </c>
       <c r="E5" t="n">
-        <v>24.59</v>
+        <v>61.28</v>
       </c>
       <c r="F5" t="n">
-        <v>33.08</v>
+        <v>101.78</v>
       </c>
       <c r="G5" t="n">
-        <v>29.44</v>
+        <v>87.34</v>
       </c>
       <c r="H5" t="n">
-        <v>19.27</v>
+        <v>68.7</v>
       </c>
       <c r="I5" t="n">
-        <v>22.68</v>
+        <v>68.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>65.08</v>
+      </c>
+      <c r="K5" t="n">
+        <v>60.48</v>
       </c>
     </row>
     <row r="6">
@@ -603,28 +637,34 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="C6" t="n">
-        <v>29.85</v>
+        <v>108.65</v>
       </c>
       <c r="D6" t="n">
-        <v>37.93</v>
+        <v>148.73</v>
       </c>
       <c r="E6" t="n">
-        <v>24.59</v>
+        <v>74.08</v>
       </c>
       <c r="F6" t="n">
-        <v>33.08</v>
+        <v>124.68</v>
       </c>
       <c r="G6" t="n">
-        <v>29.44</v>
+        <v>106.64</v>
       </c>
       <c r="H6" t="n">
-        <v>19.27</v>
+        <v>84.09999999999999</v>
       </c>
       <c r="I6" t="n">
-        <v>22.68</v>
+        <v>83.09999999999999</v>
+      </c>
+      <c r="J6" t="n">
+        <v>77.58</v>
+      </c>
+      <c r="K6" t="n">
+        <v>73.08</v>
       </c>
     </row>
     <row r="7">
@@ -634,28 +674,34 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1000</v>
+        <v>600</v>
       </c>
       <c r="C7" t="n">
-        <v>207.15</v>
+        <v>128.35</v>
       </c>
       <c r="D7" t="n">
-        <v>287.23</v>
+        <v>176.43</v>
       </c>
       <c r="E7" t="n">
-        <v>155.09</v>
+        <v>86.88</v>
       </c>
       <c r="F7" t="n">
-        <v>239.18</v>
+        <v>147.58</v>
       </c>
       <c r="G7" t="n">
-        <v>203.14</v>
+        <v>125.94</v>
       </c>
       <c r="H7" t="n">
-        <v>129.07</v>
+        <v>99.5</v>
       </c>
       <c r="I7" t="n">
-        <v>136.08</v>
+        <v>97.7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>90.08</v>
+      </c>
+      <c r="K7" t="n">
+        <v>85.68000000000001</v>
       </c>
     </row>
     <row r="8">
@@ -665,28 +711,34 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>700</v>
       </c>
       <c r="C8" t="n">
-        <v>29.85</v>
+        <v>148.05</v>
       </c>
       <c r="D8" t="n">
-        <v>37.93</v>
+        <v>204.13</v>
       </c>
       <c r="E8" t="n">
-        <v>24.59</v>
+        <v>99.68000000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>33.08</v>
+        <v>170.48</v>
       </c>
       <c r="G8" t="n">
-        <v>29.44</v>
+        <v>145.24</v>
       </c>
       <c r="H8" t="n">
-        <v>19.27</v>
+        <v>114.9</v>
       </c>
       <c r="I8" t="n">
-        <v>22.68</v>
+        <v>112.3</v>
+      </c>
+      <c r="J8" t="n">
+        <v>102.58</v>
+      </c>
+      <c r="K8" t="n">
+        <v>98.28</v>
       </c>
     </row>
     <row r="9">
@@ -696,28 +748,34 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1001</v>
+        <v>800</v>
       </c>
       <c r="C9" t="n">
-        <v>207.34</v>
+        <v>167.75</v>
       </c>
       <c r="D9" t="n">
-        <v>287.5</v>
+        <v>231.83</v>
       </c>
       <c r="E9" t="n">
-        <v>155.24</v>
+        <v>112.48</v>
       </c>
       <c r="F9" t="n">
-        <v>239.41</v>
+        <v>193.38</v>
       </c>
       <c r="G9" t="n">
-        <v>203.34</v>
+        <v>164.54</v>
       </c>
       <c r="H9" t="n">
-        <v>129.24</v>
+        <v>130.3</v>
       </c>
       <c r="I9" t="n">
-        <v>136.2</v>
+        <v>126.9</v>
+      </c>
+      <c r="J9" t="n">
+        <v>115.08</v>
+      </c>
+      <c r="K9" t="n">
+        <v>110.88</v>
       </c>
     </row>
     <row r="10">
@@ -727,28 +785,34 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="C10" t="n">
-        <v>207.15</v>
+        <v>187.45</v>
       </c>
       <c r="D10" t="n">
-        <v>287.23</v>
+        <v>259.53</v>
       </c>
       <c r="E10" t="n">
-        <v>155.09</v>
+        <v>125.28</v>
       </c>
       <c r="F10" t="n">
-        <v>239.18</v>
+        <v>216.28</v>
       </c>
       <c r="G10" t="n">
-        <v>203.14</v>
+        <v>183.84</v>
       </c>
       <c r="H10" t="n">
-        <v>129.07</v>
+        <v>145.7</v>
       </c>
       <c r="I10" t="n">
-        <v>136.08</v>
+        <v>141.5</v>
+      </c>
+      <c r="J10" t="n">
+        <v>127.58</v>
+      </c>
+      <c r="K10" t="n">
+        <v>123.48</v>
       </c>
     </row>
     <row r="11">
@@ -767,7 +831,7 @@
         <v>287.23</v>
       </c>
       <c r="E11" t="n">
-        <v>155.09</v>
+        <v>138.08</v>
       </c>
       <c r="F11" t="n">
         <v>239.18</v>
@@ -776,9 +840,15 @@
         <v>203.14</v>
       </c>
       <c r="H11" t="n">
-        <v>129.07</v>
+        <v>161.1</v>
       </c>
       <c r="I11" t="n">
+        <v>156.1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>140.07</v>
+      </c>
+      <c r="K11" t="n">
         <v>136.08</v>
       </c>
     </row>
@@ -789,28 +859,34 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="C12" t="n">
-        <v>207.15</v>
+        <v>226.85</v>
       </c>
       <c r="D12" t="n">
-        <v>287.23</v>
+        <v>314.93</v>
       </c>
       <c r="E12" t="n">
-        <v>155.09</v>
+        <v>150.88</v>
       </c>
       <c r="F12" t="n">
-        <v>239.18</v>
+        <v>262.08</v>
       </c>
       <c r="G12" t="n">
-        <v>203.14</v>
+        <v>222.44</v>
       </c>
       <c r="H12" t="n">
-        <v>129.07</v>
+        <v>171.1</v>
       </c>
       <c r="I12" t="n">
-        <v>136.08</v>
+        <v>170.7</v>
+      </c>
+      <c r="J12" t="n">
+        <v>152.57</v>
+      </c>
+      <c r="K12" t="n">
+        <v>148.68</v>
       </c>
     </row>
     <row r="13">
@@ -820,28 +896,34 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>700</v>
+        <v>1200</v>
       </c>
       <c r="C13" t="n">
-        <v>148.05</v>
+        <v>246.55</v>
       </c>
       <c r="D13" t="n">
-        <v>204.13</v>
+        <v>342.63</v>
       </c>
       <c r="E13" t="n">
-        <v>111.59</v>
+        <v>163.68</v>
       </c>
       <c r="F13" t="n">
-        <v>170.48</v>
+        <v>284.98</v>
       </c>
       <c r="G13" t="n">
-        <v>145.24</v>
+        <v>241.74</v>
       </c>
       <c r="H13" t="n">
-        <v>92.47</v>
+        <v>181.1</v>
       </c>
       <c r="I13" t="n">
-        <v>98.28</v>
+        <v>185.3</v>
+      </c>
+      <c r="J13" t="n">
+        <v>165.07</v>
+      </c>
+      <c r="K13" t="n">
+        <v>161.28</v>
       </c>
     </row>
     <row r="14">
@@ -852,25 +934,31 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="n">
-        <v>1717.69</v>
+        <v>1658.4</v>
       </c>
       <c r="D14" t="n">
-        <v>2366.73</v>
+        <v>2283.36</v>
       </c>
       <c r="E14" t="n">
-        <v>1295.73</v>
+        <v>1119.36</v>
       </c>
       <c r="F14" t="n">
-        <v>1977.29</v>
+        <v>1908.36</v>
       </c>
       <c r="G14" t="n">
-        <v>1685.18</v>
+        <v>1627.08</v>
       </c>
       <c r="H14" t="n">
-        <v>1073.21</v>
+        <v>1270.2</v>
       </c>
       <c r="I14" t="n">
-        <v>1141.68</v>
+        <v>1260</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1155.92</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1103.76</v>
       </c>
     </row>
     <row r="15">
@@ -883,6 +971,8 @@
       <c r="G15" s="1" t="inlineStr"/>
       <c r="H15" s="1" t="inlineStr"/>
       <c r="I15" s="1" t="inlineStr"/>
+      <c r="J15" s="1" t="inlineStr"/>
+      <c r="K15" s="1" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>